<commit_message>
ran a manual OF test. It all works
</commit_message>
<xml_diff>
--- a/test/test_simulation_data/Masterfile.xlsx
+++ b/test/test_simulation_data/Masterfile.xlsx
@@ -5,26 +5,26 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="main" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="par-cartesian" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="par-manual" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="par-random" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="par-output" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="main" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="par-cartesian" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="par-manual" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="par-random" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="par-output" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t xml:space="preserve">PARAMETER</t>
   </si>
@@ -41,7 +41,7 @@
     <t xml:space="preserve">mode</t>
   </si>
   <si>
-    <t xml:space="preserve">random</t>
+    <t xml:space="preserve">manual</t>
   </si>
   <si>
     <t xml:space="preserve">N_random</t>
@@ -98,9 +98,6 @@
     <t xml:space="preserve">mu</t>
   </si>
   <si>
-    <t xml:space="preserve">manual</t>
-  </si>
-  <si>
     <t xml:space="preserve">7;2</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">DISTRIBUTION</t>
@@ -153,14 +153,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -223,17 +224,41 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -248,82 +273,254 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1f497d"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="eeece1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4f818d"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="c0504d"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9bbb59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064a2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4bacc6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="f79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ff"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="51000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="20000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="5" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -332,108 +529,115 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="2" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="5" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="5" t="n">
         <v>500</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="5" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -442,66 +646,81 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="7" width="12.43"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B3" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>11412</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>11412</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="5" t="n">
+        <v>123214</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>123214</v>
+      <c r="B5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>123512</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -510,89 +729,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="20.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="20.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="5" t="n">
         <v>20000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -601,62 +822,63 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>